<commit_message>
Sesion ----------- Cambio el tipo de dato del PIN de int a string.
Transaccion
-----------
Se decidio un implementación más sencilla, pero más estática eliminando los tipos de comportamiento.

Se decidió generar un atributo estático para el cálculo de la secuencia en las transacciones.

Dinero
-----------
Se crearon dos métodos: Agregar y Quitar para que modifique el estado del dinero almacenado en Caja.
</commit_message>
<xml_diff>
--- a/ATM/Estado de objetos ATM.xlsx
+++ b/ATM/Estado de objetos ATM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="660" windowWidth="25360" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>CLASES</t>
   </si>
@@ -133,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -189,7 +195,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -205,8 +211,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -215,8 +225,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -224,6 +235,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -231,6 +244,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,7 +578,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -625,14 +640,14 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3">
@@ -642,20 +657,22 @@
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3">
@@ -667,64 +684,64 @@
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2"/>
@@ -735,8 +752,8 @@
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2"/>
@@ -759,7 +776,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>